<commit_message>
Fix: Fixed padding colouring
</commit_message>
<xml_diff>
--- a/pandas_xlsxwriter.xlsx
+++ b/pandas_xlsxwriter.xlsx
@@ -1,23 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricks\OneDrive\Development\Tools\cgdat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_44301ABBE865B41F28EF4AE9692E6EF986399E00" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{02F17325-BAA7-427E-AF39-2960623423DE}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_095C0E466BC0C4E23F08E79DF69BCA67F9CEE6E9" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{14152B28-FD43-4F2C-803E-E6CA9C83E5F5}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="condition_color_bool" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -31,24 +46,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -63,15 +66,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -416,100 +427,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:B13"/>
+  <dimension ref="A3:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="B10">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>9</v>
-      </c>
-      <c r="B12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="B13">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -519,7 +470,7 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="1" id="{00000000-000E-0000-0000-000001000000}">
-            <xm:f>condition_color_bool!$A1=TRUE</xm:f>
+            <xm:f>Sheet2!A1="a"</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF006100"/>
@@ -531,7 +482,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A3:B13</xm:sqref>
+          <xm:sqref>A3:A8</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -541,67 +492,125 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A3:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{00000000-000E-0000-0100-000001000000}">
+            <xm:f>Sheet2!B1="a"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>A3:A8</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="b">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="b">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="b">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="b">
-        <v>1</v>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>